<commit_message>
Atualização das notas do resumo da aula 04
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce747\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13050848-18B4-47C8-87F4-2061022CB1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC4DCF9-E795-4DF2-8716-2017ED9FC28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{72A12B66-DA0A-4AA8-A080-AA2CD399E4D5}"/>
   </bookViews>
@@ -773,13 +773,13 @@
   <dimension ref="A4:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="13" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -1155,7 +1155,8 @@
         <v>43</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <f>CEILING(95*0.8,1)</f>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1481,6 +1482,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="ATYnjeXuTgQD2UyJhQoGsTj1/SsuuzgFBWofSq39VklkFdK7fpScCh8+UhwaRKq+tefdqtP1SizSWPdZi8A/qg==" saltValue="g7N6G03JlFuoKOlMMMXhqA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Notas do resumo da aula 06
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce747\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC4DCF9-E795-4DF2-8716-2017ED9FC28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B64B9E3-65C6-422C-8D1C-2532491668F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{72A12B66-DA0A-4AA8-A080-AA2CD399E4D5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Resumos" sheetId="1" r:id="rId1"/>
     <sheet name="Seminários" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
   <si>
     <t>Matrícula</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>Aula 27</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
   <dimension ref="A4:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,6 +837,10 @@
       <c r="C5" s="3">
         <v>87</v>
       </c>
+      <c r="D5" s="3">
+        <f>CEILING(90*0.8,1)</f>
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -845,7 +852,9 @@
       <c r="C6" s="4">
         <v>97</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -866,6 +875,9 @@
       <c r="C7" s="3">
         <v>83</v>
       </c>
+      <c r="D7" s="3">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -877,7 +889,9 @@
       <c r="C8" s="4">
         <v>92</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>90</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -898,6 +912,9 @@
       <c r="C9" s="3">
         <v>98</v>
       </c>
+      <c r="D9" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -909,7 +926,9 @@
       <c r="C10" s="4">
         <v>96</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -930,6 +949,9 @@
       <c r="C11" s="3">
         <v>95</v>
       </c>
+      <c r="D11" s="3">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -938,10 +960,12 @@
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -962,6 +986,9 @@
       <c r="C13" s="3">
         <v>89</v>
       </c>
+      <c r="D13" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -973,7 +1000,9 @@
       <c r="C14" s="4">
         <v>27</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -994,6 +1023,10 @@
       <c r="C15" s="3">
         <v>98</v>
       </c>
+      <c r="D15" s="3">
+        <f>CEILING(97*0.8,1)</f>
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1005,7 +1038,9 @@
       <c r="C16" s="4">
         <v>0</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4">
+        <v>91</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1026,6 +1061,9 @@
       <c r="C17" s="3">
         <v>94</v>
       </c>
+      <c r="D17" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1037,7 +1075,10 @@
       <c r="C18" s="4">
         <v>97</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4">
+        <f>CEILING(91*0.9,1)</f>
+        <v>82</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1059,6 +1100,9 @@
         <f>CEILING(92*0.8,1)</f>
         <v>74</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1070,7 +1114,9 @@
       <c r="C20" s="4">
         <v>92</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4">
+        <v>88</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1092,6 +1138,9 @@
         <f>CEILING(94*0.9,1)</f>
         <v>85</v>
       </c>
+      <c r="D21" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1104,7 +1153,9 @@
         <f>CEILING(85*0.9,1)</f>
         <v>77</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4">
+        <v>86</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1125,6 +1176,9 @@
       <c r="C23" s="3">
         <v>91</v>
       </c>
+      <c r="D23" s="3">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1136,7 +1190,9 @@
       <c r="C24" s="4">
         <v>93</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="4">
+        <v>92</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1158,6 +1214,10 @@
         <f>CEILING(95*0.8,1)</f>
         <v>76</v>
       </c>
+      <c r="D25" s="3">
+        <f>CEILING(92*0.7,1)</f>
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1170,7 +1230,9 @@
         <f>CEILING(93*0.9,1)</f>
         <v>84</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4">
+        <v>97</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1191,6 +1253,9 @@
       <c r="C27" s="3">
         <v>96</v>
       </c>
+      <c r="D27" s="3">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1202,7 +1267,9 @@
       <c r="C28" s="4">
         <v>100</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4">
+        <v>98</v>
+      </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1223,6 +1290,9 @@
       <c r="C29" s="3">
         <v>68</v>
       </c>
+      <c r="D29" s="3">
+        <v>89</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1234,7 +1304,9 @@
       <c r="C30" s="4">
         <v>100</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4">
+        <v>93</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1256,6 +1328,9 @@
         <f>CEILING(93*0.9,1)</f>
         <v>84</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1264,10 +1339,12 @@
       <c r="B32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1288,6 +1365,10 @@
       <c r="C33" s="3">
         <v>78</v>
       </c>
+      <c r="D33" s="3">
+        <f>CEILING(81*0.7,1)</f>
+        <v>57</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1299,7 +1380,9 @@
       <c r="C34" s="4">
         <v>99</v>
       </c>
-      <c r="D34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1320,6 +1403,9 @@
       <c r="C35" s="3">
         <v>91</v>
       </c>
+      <c r="D35" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1328,10 +1414,12 @@
       <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="4">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1352,6 +1440,9 @@
       <c r="C37" s="3">
         <v>94</v>
       </c>
+      <c r="D37" s="3">
+        <v>84</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1363,7 +1454,9 @@
       <c r="C38" s="4">
         <v>89</v>
       </c>
-      <c r="D38" s="4"/>
+      <c r="D38" s="4">
+        <v>90</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1384,6 +1477,9 @@
       <c r="C39" s="3">
         <v>81</v>
       </c>
+      <c r="D39" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1395,7 +1491,9 @@
       <c r="C40" s="4">
         <v>88</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="4">
+        <v>96</v>
+      </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1416,6 +1514,10 @@
       <c r="C41" s="3">
         <v>95</v>
       </c>
+      <c r="D41" s="3">
+        <f>CEILING(97*0.9,1)</f>
+        <v>88</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1427,7 +1529,9 @@
       <c r="C42" s="4">
         <v>82</v>
       </c>
-      <c r="D42" s="4"/>
+      <c r="D42" s="4">
+        <v>54</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1448,6 +1552,9 @@
       <c r="C43" s="3">
         <v>87</v>
       </c>
+      <c r="D43" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1459,7 +1566,9 @@
       <c r="C44" s="4">
         <v>91</v>
       </c>
-      <c r="D44" s="4"/>
+      <c r="D44" s="4">
+        <v>91</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1480,9 +1589,12 @@
       <c r="C45" s="3">
         <v>0</v>
       </c>
+      <c r="D45" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ATYnjeXuTgQD2UyJhQoGsTj1/SsuuzgFBWofSq39VklkFdK7fpScCh8+UhwaRKq+tefdqtP1SizSWPdZi8A/qg==" saltValue="g7N6G03JlFuoKOlMMMXhqA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yKTPyuhl2xsINr9x1Xo0XEgxwtjPHWL5CQPK+mOHaZYLY69C8DluFRw0OkWqOOiHzdJrB1WMTbbBAIUIeRLidA==" saltValue="+2czRtRpVY6xYUDh5wISjQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Notas para os resumos das aulas 8 e 10
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce747\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B64B9E3-65C6-422C-8D1C-2532491668F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306A34FF-0EBD-4FC3-8CF4-0F4B3152D176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{72A12B66-DA0A-4AA8-A080-AA2CD399E4D5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>Iago Augusto</author>
   </authors>
   <commentList>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{D313E3B9-3ECC-4BC0-B56A-701693D1B7A1}">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{D313E3B9-3ECC-4BC0-B56A-701693D1B7A1}">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{59ABBED4-D084-46AB-A19E-3E54127CE42C}">
+    <comment ref="B45" authorId="0" shapeId="0" xr:uid="{59ABBED4-D084-46AB-A19E-3E54127CE42C}">
       <text>
         <r>
           <rPr>
@@ -91,258 +91,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>Matrícula</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>2017.1.08.046</t>
   </si>
   <si>
-    <t>Alice Batista Nogueira</t>
-  </si>
-  <si>
     <t>2017.1.08.036</t>
   </si>
   <si>
-    <t>Augusto Georges Adao Miotti</t>
-  </si>
-  <si>
     <t>2021.1.08.029</t>
   </si>
   <si>
-    <t>Betania Lopes Silva Marques</t>
-  </si>
-  <si>
     <t>2019.1.08.042</t>
   </si>
   <si>
-    <t>Bruna Pereira Falcucci</t>
-  </si>
-  <si>
     <t>2019.1.08.032</t>
   </si>
   <si>
-    <t>Caio Marinello Moura Leite</t>
-  </si>
-  <si>
     <t>2017.1.08.017</t>
   </si>
   <si>
-    <t>Carlos Eduardo Pavão Aureliano</t>
-  </si>
-  <si>
     <t>2019.1.08.019</t>
   </si>
   <si>
-    <t>Douglas Felipe de Morais</t>
-  </si>
-  <si>
     <t>2018.1.08.026</t>
   </si>
   <si>
-    <t>Eduardo Guerreiro Rocha</t>
-  </si>
-  <si>
     <t>2019.1.08.003</t>
   </si>
   <si>
-    <t>Eduardo Sapio Saccardo</t>
-  </si>
-  <si>
     <t>2018.1.08.013</t>
   </si>
   <si>
-    <t>Felipe Martins Choi</t>
-  </si>
-  <si>
     <t>2019.1.08.005</t>
   </si>
   <si>
-    <t>Gabriel Takahiro Toma de Lima</t>
-  </si>
-  <si>
     <t>2018.1.08.049</t>
   </si>
   <si>
-    <t>Gustavo Celestino de Lima</t>
-  </si>
-  <si>
     <t>2017.1.08.022</t>
   </si>
   <si>
-    <t>Gustavo Moreira Penna</t>
-  </si>
-  <si>
     <t>2018.1.08.048</t>
   </si>
   <si>
-    <t>Hugo José Teodoro Terra</t>
-  </si>
-  <si>
     <t>2015.1.08.028</t>
   </si>
   <si>
-    <t>Iago Vinicius Siqueira Ribeiro</t>
-  </si>
-  <si>
     <t>2019.1.08.030</t>
   </si>
   <si>
-    <t>Isabelle Sgrignero</t>
-  </si>
-  <si>
     <t>2020.1.08.023</t>
   </si>
   <si>
-    <t>Jasmine Germano França</t>
-  </si>
-  <si>
     <t>2018.1.08.028</t>
   </si>
   <si>
-    <t>Jean Vitor da Silva</t>
-  </si>
-  <si>
     <t>2019.1.08.010</t>
   </si>
   <si>
-    <t>João Pedro Silva Bianco</t>
-  </si>
-  <si>
     <t>2021.1.08.010</t>
   </si>
   <si>
-    <t>Joao Vitor Azevedo Vigarani</t>
-  </si>
-  <si>
     <t>2021.1.08.011</t>
   </si>
   <si>
-    <t>Jose Argemiro dos Reis Neto</t>
-  </si>
-  <si>
     <t>2017.1.08.044</t>
   </si>
   <si>
-    <t>Leonardo Pessoa Oliveira Alves</t>
-  </si>
-  <si>
     <t>2018.1.08.040</t>
   </si>
   <si>
-    <t>Luana de Jesus Carvalho</t>
-  </si>
-  <si>
     <t>2018.1.08.009</t>
   </si>
   <si>
-    <t>Lucas Bertoni Scarton</t>
-  </si>
-  <si>
     <t>2018.1.08.047</t>
   </si>
   <si>
-    <t>Lucas da Silva Justino</t>
-  </si>
-  <si>
     <t>2020.1.08.026</t>
   </si>
   <si>
-    <t>Lucas Dogo de Souza Pezzuto</t>
-  </si>
-  <si>
     <t>2017.1.08.034</t>
   </si>
   <si>
-    <t>Lúcio de Moura Peloso</t>
-  </si>
-  <si>
     <t>2017.1.08.039</t>
   </si>
   <si>
-    <t>Marcus Vinicius Garcia Miguel</t>
-  </si>
-  <si>
     <t>2018.1.08.030</t>
   </si>
   <si>
-    <t>Maria Eduarda Santos Silva</t>
-  </si>
-  <si>
     <t>2020.1.08.025</t>
   </si>
   <si>
-    <t>Matheus Malvao Barbosa</t>
-  </si>
-  <si>
     <t>2019.1.08.015</t>
   </si>
   <si>
-    <t>Murilo Sousa Moraes</t>
-  </si>
-  <si>
     <t>2017.1.08.026</t>
   </si>
   <si>
-    <t>Natália Machado dos Santos</t>
-  </si>
-  <si>
     <t>2018.1.08.041</t>
   </si>
   <si>
-    <t>Otávio Augusto Marcelino Izidoro</t>
-  </si>
-  <si>
     <t>2018.1.08.046</t>
   </si>
   <si>
-    <t>Paulo Emilio Godinho da Fonseca</t>
-  </si>
-  <si>
     <t>2017.1.08.031</t>
   </si>
   <si>
-    <t>Pedro Bortolin</t>
-  </si>
-  <si>
     <t>2019.1.08.016</t>
   </si>
   <si>
-    <t>Renê Augusto de Souza</t>
-  </si>
-  <si>
     <t>2018.1.08.042</t>
   </si>
   <si>
-    <t>Rodrigo Silva de Paulo</t>
-  </si>
-  <si>
     <t>2020.1.08.018</t>
   </si>
   <si>
-    <t>Victor Hugo Tozzo Filho</t>
-  </si>
-  <si>
     <t>2021.1.08.023</t>
   </si>
   <si>
-    <t>Victor Ribeiro Gonçalez</t>
-  </si>
-  <si>
     <t>2019.1.08.017</t>
   </si>
   <si>
-    <t>Vitor Reis Rubatino</t>
-  </si>
-  <si>
     <t>2016.1.08.037</t>
-  </si>
-  <si>
-    <t>Vitor Risso Parisi</t>
   </si>
   <si>
     <t>Aula 04</t>
@@ -773,89 +647,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03278D3-56F1-453D-BD81-7624E822CB85}">
-  <dimension ref="A4:M45"/>
+  <dimension ref="A4:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="13" width="8.88671875" style="3"/>
+    <col min="2" max="12" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="B5" s="3">
         <v>87</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
       <c r="C5" s="3">
-        <v>87</v>
-      </c>
-      <c r="D5" s="3">
         <f>CEILING(90*0.8,1)</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D5" s="3">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
         <v>97</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="4">
+        <v>92</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -863,36 +738,41 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>83</v>
       </c>
       <c r="C7" s="3">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D7" s="3">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <f>CEILING(95*0.9,1)</f>
+        <v>86</v>
+      </c>
+      <c r="E7" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>92</v>
       </c>
       <c r="C8" s="4">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="4">
-        <v>90</v>
-      </c>
-      <c r="E8" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -900,36 +780,42 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>98</v>
       </c>
       <c r="C9" s="3">
+        <v>95</v>
+      </c>
+      <c r="D9" s="3">
+        <v>94</v>
+      </c>
+      <c r="E9" s="3">
+        <f>CEILING(100*0.9,1)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>96</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="4">
+        <f>CEILING(91*0.8,1)</f>
+        <v>73</v>
+      </c>
+      <c r="E10" s="4">
         <v>98</v>
       </c>
-      <c r="D9" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4">
-        <v>96</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -937,36 +823,40 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
+        <v>95</v>
       </c>
       <c r="C11" s="3">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D11" s="3">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E11" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -974,36 +864,41 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3">
+        <v>89</v>
       </c>
       <c r="C13" s="3">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D13" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
         <v>27</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E14" s="4">
+        <f>CEILING(96*0.9,1)</f>
+        <v>87</v>
+      </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1011,37 +906,42 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <v>98</v>
       </c>
       <c r="C15" s="3">
-        <v>98</v>
-      </c>
-      <c r="D15" s="3">
         <f>CEILING(97*0.8,1)</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="3">
+        <v>97</v>
+      </c>
+      <c r="E15" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
       </c>
       <c r="C16" s="4">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="D16" s="4">
-        <v>91</v>
-      </c>
-      <c r="E16" s="4"/>
+        <f>CEILING(93*0.9,1)</f>
+        <v>84</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -1049,37 +949,41 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3">
+        <v>94</v>
       </c>
       <c r="C17" s="3">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="4">
+        <v>97</v>
       </c>
       <c r="C18" s="4">
-        <v>97</v>
-      </c>
-      <c r="D18" s="4">
         <f>CEILING(91*0.9,1)</f>
         <v>82</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="4">
+        <v>90</v>
+      </c>
+      <c r="E18" s="4">
+        <v>95</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1087,37 +991,41 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="3">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
         <f>CEILING(92*0.8,1)</f>
         <v>74</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4">
+        <v>88</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="4">
         <v>95</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="4">
-        <v>92</v>
-      </c>
-      <c r="D20" s="4">
-        <v>88</v>
-      </c>
-      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1125,38 +1033,43 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3">
+        <v>17</v>
+      </c>
+      <c r="B21" s="3">
         <f>CEILING(94*0.9,1)</f>
         <v>85</v>
       </c>
+      <c r="C21" s="3">
+        <v>86</v>
+      </c>
       <c r="D21" s="3">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E21" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="4">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4">
         <f>CEILING(85*0.9,1)</f>
         <v>77</v>
       </c>
-      <c r="D22" s="4">
+      <c r="C22" s="4">
         <v>86</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="4">
+        <f>CEILING(80*0.7,1)</f>
+        <v>56</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1164,36 +1077,40 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <v>91</v>
       </c>
       <c r="C23" s="3">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D23" s="3">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E23" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="B24" s="4">
+        <v>93</v>
       </c>
       <c r="C24" s="4">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="4">
         <v>92</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1201,39 +1118,43 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="3">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3">
         <f>CEILING(95*0.8,1)</f>
         <v>76</v>
       </c>
-      <c r="D25" s="3">
+      <c r="C25" s="3">
         <f>CEILING(92*0.7,1)</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="4">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4">
         <f>CEILING(93*0.9,1)</f>
         <v>84</v>
       </c>
+      <c r="C26" s="4">
+        <v>97</v>
+      </c>
       <c r="D26" s="4">
-        <v>97</v>
-      </c>
-      <c r="E26" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1241,36 +1162,41 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
+        <v>23</v>
+      </c>
+      <c r="B27" s="3">
+        <v>96</v>
       </c>
       <c r="C27" s="3">
-        <v>96</v>
-      </c>
-      <c r="D27" s="3">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="3">
+        <f>CEILING(91*0.8,1)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="B28" s="4">
+        <v>100</v>
       </c>
       <c r="C28" s="4">
+        <v>98</v>
+      </c>
+      <c r="D28" s="4">
         <v>100</v>
       </c>
-      <c r="D28" s="4">
-        <v>98</v>
-      </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1278,36 +1204,41 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="B29" s="3">
+        <v>68</v>
       </c>
       <c r="C29" s="3">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="E29" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
+      </c>
+      <c r="B30" s="4">
+        <v>100</v>
       </c>
       <c r="C30" s="4">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D30" s="4">
-        <v>93</v>
-      </c>
-      <c r="E30" s="4"/>
+        <f>CEILING(89*0.9,1)</f>
+        <v>81</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -1315,37 +1246,42 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="3">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3">
         <f>CEILING(93*0.9,1)</f>
         <v>84</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="3">
+        <v>90</v>
+      </c>
+      <c r="E31" s="3">
+        <f>CEILING(95*0.9,1)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E32" s="4">
+        <v>75</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1353,37 +1289,42 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="B33" s="3">
+        <v>78</v>
       </c>
       <c r="C33" s="3">
-        <v>78</v>
-      </c>
-      <c r="D33" s="3">
         <f>CEILING(81*0.7,1)</f>
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D33" s="3">
+        <v>81</v>
+      </c>
+      <c r="E33" s="3">
+        <f>CEILING(82*0.9,1)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="4">
+        <v>30</v>
+      </c>
+      <c r="B34" s="4">
         <v>99</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="4">
+        <v>90</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -1391,36 +1332,41 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>63</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="3">
+        <v>91</v>
       </c>
       <c r="C35" s="3">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D35" s="3">
         <v>86</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E35" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E36" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="E36" s="4">
+        <f>CEILING(97*0.8,1)</f>
+        <v>78</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -1428,36 +1374,40 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
+        <v>33</v>
+      </c>
+      <c r="B37" s="3">
+        <v>94</v>
       </c>
       <c r="C37" s="3">
+        <v>84</v>
+      </c>
+      <c r="D37" s="3">
+        <v>88</v>
+      </c>
+      <c r="E37" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="4">
+        <v>89</v>
+      </c>
+      <c r="C38" s="4">
+        <v>90</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="4">
         <v>94</v>
       </c>
-      <c r="D37" s="3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="4">
-        <v>89</v>
-      </c>
-      <c r="D38" s="4">
-        <v>90</v>
-      </c>
-      <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -1465,36 +1415,40 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="3">
+        <v>35</v>
+      </c>
+      <c r="B39" s="3">
         <v>81</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="3">
+        <v>90</v>
+      </c>
+      <c r="E39" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>36</v>
+      </c>
+      <c r="B40" s="4">
+        <v>88</v>
       </c>
       <c r="C40" s="4">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D40" s="4">
-        <v>96</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="E40" s="4">
+        <v>92</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -1502,37 +1456,42 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
+        <v>37</v>
+      </c>
+      <c r="B41" s="3">
+        <v>95</v>
       </c>
       <c r="C41" s="3">
-        <v>95</v>
-      </c>
-      <c r="D41" s="3">
         <f>CEILING(97*0.9,1)</f>
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D41" s="3">
+        <v>91</v>
+      </c>
+      <c r="E41" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="4">
+        <v>82</v>
+      </c>
+      <c r="C42" s="4">
+        <v>54</v>
+      </c>
+      <c r="D42" s="4">
+        <v>88</v>
+      </c>
+      <c r="E42" s="4">
+        <f>CEILING(94*0.8,1)</f>
         <v>76</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="4">
-        <v>82</v>
-      </c>
-      <c r="D42" s="4">
-        <v>54</v>
-      </c>
-      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -1540,36 +1499,41 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" t="s">
-        <v>79</v>
+        <v>39</v>
+      </c>
+      <c r="B43" s="3">
+        <v>87</v>
       </c>
       <c r="C43" s="3">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D43" s="3">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E43" s="3">
+        <f>CEILING(90*0.9,1)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>81</v>
+        <v>40</v>
+      </c>
+      <c r="B44" s="4">
+        <v>91</v>
       </c>
       <c r="C44" s="4">
         <v>91</v>
       </c>
-      <c r="D44" s="4">
-        <v>91</v>
-      </c>
-      <c r="E44" s="4"/>
+      <c r="D44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="4">
+        <v>86</v>
+      </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -1577,24 +1541,25 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="3">
+        <v>41</v>
+      </c>
+      <c r="B45" s="3">
         <v>0</v>
       </c>
+      <c r="C45" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D45" s="3" t="s">
-        <v>95</v>
+        <v>53</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yKTPyuhl2xsINr9x1Xo0XEgxwtjPHWL5CQPK+mOHaZYLY69C8DluFRw0OkWqOOiHzdJrB1WMTbbBAIUIeRLidA==" saltValue="+2czRtRpVY6xYUDh5wISjQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Notas do resumo da aula 12
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce747\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306A34FF-0EBD-4FC3-8CF4-0F4B3152D176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4223321D-26F4-4561-BB17-3A75E23DCE58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{72A12B66-DA0A-4AA8-A080-AA2CD399E4D5}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Seminários" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -91,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Matrícula</t>
   </si>
@@ -649,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03278D3-56F1-453D-BD81-7624E822CB85}">
   <dimension ref="A4:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,6 +716,9 @@
       <c r="E5" s="3">
         <v>78</v>
       </c>
+      <c r="F5" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -731,7 +736,10 @@
       <c r="E6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <f>CEILING(85*0.9,1)</f>
+        <v>77</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -756,6 +764,9 @@
       <c r="E7" s="3">
         <v>92</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -773,7 +784,9 @@
       <c r="E8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -798,6 +811,9 @@
         <f>CEILING(100*0.9,1)</f>
         <v>90</v>
       </c>
+      <c r="F9" s="3">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -816,7 +832,9 @@
       <c r="E10" s="4">
         <v>98</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <v>91</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -840,6 +858,9 @@
       <c r="E11" s="3">
         <v>90</v>
       </c>
+      <c r="F11" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -857,7 +878,9 @@
       <c r="E12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -881,6 +904,9 @@
       <c r="E13" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F13" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -899,7 +925,9 @@
         <f>CEILING(96*0.9,1)</f>
         <v>87</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -924,6 +952,9 @@
       <c r="E15" s="3">
         <v>98</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -942,7 +973,10 @@
       <c r="E16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4">
+        <f>CEILING(57*0.3,1)</f>
+        <v>18</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -966,6 +1000,9 @@
       <c r="E17" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F17" s="3">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -984,7 +1021,10 @@
       <c r="E18" s="4">
         <v>95</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4">
+        <f>CEILING(100*0.9,1)</f>
+        <v>90</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1009,6 +1049,9 @@
       <c r="E19" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1026,7 +1069,9 @@
       <c r="E20" s="4">
         <v>95</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="4">
+        <v>96</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1051,6 +1096,9 @@
       <c r="E21" s="3">
         <v>91</v>
       </c>
+      <c r="F21" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1070,7 +1118,9 @@
         <f>CEILING(80*0.7,1)</f>
         <v>56</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4">
+        <v>81</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1094,6 +1144,10 @@
       <c r="E23" s="3">
         <v>93</v>
       </c>
+      <c r="F23" s="3">
+        <f>CEILING(92*0.9,1)</f>
+        <v>83</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1111,7 +1165,9 @@
       <c r="E24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1137,6 +1193,9 @@
       <c r="E25" s="3">
         <v>90</v>
       </c>
+      <c r="F25" s="3">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1155,7 +1214,9 @@
       <c r="E26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="4">
+        <v>88</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1180,6 +1241,9 @@
         <f>CEILING(91*0.8,1)</f>
         <v>73</v>
       </c>
+      <c r="F27" s="3">
+        <v>87</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1197,7 +1261,9 @@
       <c r="E28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4">
+        <v>99</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1221,6 +1287,9 @@
       <c r="E29" s="3">
         <v>87</v>
       </c>
+      <c r="F29" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -1239,7 +1308,9 @@
       <c r="E30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="4">
+        <v>94</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -1265,6 +1336,9 @@
         <f>CEILING(95*0.9,1)</f>
         <v>86</v>
       </c>
+      <c r="F31" s="3">
+        <v>92</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
@@ -1282,7 +1356,9 @@
       <c r="E32" s="4">
         <v>75</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="4">
+        <v>93</v>
+      </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1308,6 +1384,9 @@
         <f>CEILING(82*0.9,1)</f>
         <v>74</v>
       </c>
+      <c r="F33" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1325,7 +1404,9 @@
       <c r="E34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="4">
+        <v>95</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -1349,6 +1430,9 @@
       <c r="E35" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F35" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1367,7 +1451,10 @@
         <f>CEILING(97*0.8,1)</f>
         <v>78</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="4">
+        <f>CEILING(87*0.9,1)</f>
+        <v>79</v>
+      </c>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1391,6 +1478,9 @@
       <c r="E37" s="3">
         <v>90</v>
       </c>
+      <c r="F37" s="3">
+        <v>95</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1408,7 +1498,9 @@
       <c r="E38" s="4">
         <v>94</v>
       </c>
-      <c r="F38" s="4"/>
+      <c r="F38" s="4">
+        <v>94</v>
+      </c>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -1432,6 +1524,9 @@
       <c r="E39" s="3">
         <v>83</v>
       </c>
+      <c r="F39" s="3">
+        <v>86</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1449,7 +1544,9 @@
       <c r="E40" s="4">
         <v>92</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -1474,6 +1571,9 @@
       <c r="E41" s="3">
         <v>92</v>
       </c>
+      <c r="F41" s="3">
+        <v>94</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1492,7 +1592,10 @@
         <f>CEILING(94*0.8,1)</f>
         <v>76</v>
       </c>
-      <c r="F42" s="4"/>
+      <c r="F42" s="4">
+        <f>CEILING(85*0.8,1)</f>
+        <v>68</v>
+      </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -1517,6 +1620,9 @@
         <f>CEILING(90*0.9,1)</f>
         <v>81</v>
       </c>
+      <c r="F43" s="3">
+        <v>93</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1534,7 +1640,9 @@
       <c r="E44" s="4">
         <v>86</v>
       </c>
-      <c r="F44" s="4"/>
+      <c r="F44" s="4">
+        <v>97</v>
+      </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
@@ -1556,6 +1664,9 @@
         <v>53</v>
       </c>
       <c r="E45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>